<commit_message>
added -add doctor, -print patients list per doctor, -no pressure in input parameters while patient signing
</commit_message>
<xml_diff>
--- a/records/card.xlsx
+++ b/records/card.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LotusApp\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42CE23-6242-4CF5-ACB1-4C304F4B0B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D60D50E-A3EC-4E46-97F6-5DE0676DF1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="550" windowWidth="9810" windowHeight="9530" xr2:uid="{A023F955-0644-49A9-A45C-03578E6405F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{A023F955-0644-49A9-A45C-03578E6405F0}"/>
   </bookViews>
   <sheets>
     <sheet name="form" sheetId="1" r:id="rId1"/>
+    <sheet name="list" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">form!$A$1:$I$49</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Карточка пациента </t>
   </si>
@@ -76,6 +77,24 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>doc id=</t>
+  </si>
+  <si>
+    <t>doc_name</t>
+  </si>
+  <si>
+    <t>patient num</t>
+  </si>
+  <si>
+    <t>patient name</t>
+  </si>
+  <si>
+    <t>М\Ж\Р</t>
+  </si>
+  <si>
+    <t>Дата рождения</t>
   </si>
 </sst>
 </file>
@@ -490,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8461DACE-C7F6-4328-BA3B-0FC980EBB09B}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -697,4 +716,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8EC786-03C6-4B83-8AC3-5E19F6AD228C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>